<commit_message>
phase 1 bug fixed
</commit_message>
<xml_diff>
--- a/Power Supply Design/Calc_v2.xlsx
+++ b/Power Supply Design/Calc_v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank-Desktop\git\power_electronics\Power Supply Design\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Frank-Laptop\git\power_electronics\Power Supply Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="348">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="349">
   <si>
     <t>Given specifications</t>
   </si>
@@ -1086,6 +1086,9 @@
   </si>
   <si>
     <t>H.A</t>
+  </si>
+  <si>
+    <t>Ohm.m</t>
   </si>
 </sst>
 </file>
@@ -1523,8 +1526,8 @@
   </sheetPr>
   <dimension ref="A1:L468"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A444" zoomScale="145" zoomScaleNormal="100" zoomScaleSheetLayoutView="145" workbookViewId="0">
-      <selection activeCell="B454" sqref="B454"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A281" zoomScale="130" zoomScaleNormal="100" zoomScaleSheetLayoutView="130" workbookViewId="0">
+      <selection activeCell="D292" sqref="D292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4046,7 +4049,7 @@
         <v>1.6779999999999999E-8</v>
       </c>
       <c r="D291" s="29" t="s">
-        <v>205</v>
+        <v>348</v>
       </c>
       <c r="E291" s="9"/>
       <c r="G291" s="2"/>

</xml_diff>